<commit_message>
names updated in Olivier's code
</commit_message>
<xml_diff>
--- a/v13_newUI/www/data/parameters - backup both names.xlsx
+++ b/v13_newUI/www/data/parameters - backup both names.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\App\www\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\IBM project_Sai\RAI model\v13_newUI\www\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="212">
   <si>
     <t>Baseline</t>
   </si>
@@ -654,6 +654,12 @@
   </si>
   <si>
     <t>tm_3</t>
+  </si>
+  <si>
+    <t>RCDthresh</t>
+  </si>
+  <si>
+    <t>Upper limit on annual incidence per 1000 for RCD</t>
   </si>
 </sst>
 </file>
@@ -698,12 +704,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -852,7 +864,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -866,6 +878,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1022,8 +1035,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L54" totalsRowShown="0">
-  <autoFilter ref="A1:L54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L55" totalsRowShown="0">
+  <autoFilter ref="A1:L55"/>
   <tableColumns count="12">
     <tableColumn id="1" name="category"/>
     <tableColumn id="2" name="sub_category"/>
@@ -1364,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2321,35 +2334,33 @@
       <c r="B27" t="s">
         <v>31</v>
       </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
+      <c r="C27" s="7"/>
       <c r="D27" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>211</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>82</v>
+        <v>211</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>211</v>
       </c>
       <c r="H27">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="I27" t="s">
         <v>147</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="L27">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2360,34 +2371,34 @@
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H28">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="I28" t="s">
         <v>147</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2398,25 +2409,34 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>93</v>
+        <v>147</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>8</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2427,34 +2447,25 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H30">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>147</v>
-      </c>
-      <c r="J30">
-        <v>5</v>
-      </c>
-      <c r="K30">
-        <v>200</v>
-      </c>
-      <c r="L30">
-        <v>5</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2465,34 +2476,34 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H31">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I31" t="s">
         <v>147</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K31">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L31">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2503,34 +2514,34 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H32">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I32" t="s">
         <v>147</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32">
         <v>100</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2541,34 +2552,34 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E33" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G33" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H33">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="I33" t="s">
         <v>147</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33">
         <v>100</v>
       </c>
       <c r="L33">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2579,22 +2590,22 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H34">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="I34" t="s">
         <v>147</v>
@@ -2606,7 +2617,7 @@
         <v>100</v>
       </c>
       <c r="L34">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2617,22 +2628,22 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H35">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="I35" t="s">
         <v>147</v>
@@ -2655,22 +2666,22 @@
         <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I36" t="s">
         <v>147</v>
@@ -2690,25 +2701,37 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="D37" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="E37" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="G37" t="s">
-        <v>51</v>
-      </c>
-      <c r="H37" t="b">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>147</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>100</v>
+      </c>
+      <c r="L37">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2719,34 +2742,22 @@
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="D38" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E38" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="G38" t="s">
-        <v>96</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38" t="s">
-        <v>147</v>
-      </c>
-      <c r="J38">
-        <v>0.25</v>
-      </c>
-      <c r="K38">
-        <v>3</v>
-      </c>
-      <c r="L38">
-        <v>0.25</v>
+        <v>51</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2757,34 +2768,34 @@
         <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H39">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="I39" t="s">
         <v>147</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K39">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="L39">
-        <v>5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2792,25 +2803,37 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="D40" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E40" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="G40" t="s">
-        <v>52</v>
-      </c>
-      <c r="H40" t="b">
-        <v>0</v>
+        <v>97</v>
+      </c>
+      <c r="H40">
+        <v>90</v>
+      </c>
+      <c r="I40" t="s">
+        <v>147</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>90</v>
+      </c>
+      <c r="L40">
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2821,34 +2844,22 @@
         <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="D41" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E41" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="G41" t="s">
-        <v>98</v>
-      </c>
-      <c r="H41">
-        <v>2</v>
-      </c>
-      <c r="I41" t="s">
-        <v>147</v>
-      </c>
-      <c r="J41">
-        <v>0.25</v>
-      </c>
-      <c r="K41">
-        <v>3</v>
-      </c>
-      <c r="L41">
-        <v>0.25</v>
+        <v>52</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2859,34 +2870,34 @@
         <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H42">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="I42" t="s">
         <v>147</v>
       </c>
       <c r="J42">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K42">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="L42">
-        <v>10</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2897,22 +2908,22 @@
         <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D43" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="E43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H43">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="I43" t="s">
         <v>147</v>
@@ -2924,7 +2935,7 @@
         <v>100</v>
       </c>
       <c r="L43">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2935,22 +2946,22 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H44">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="I44" t="s">
         <v>147</v>
@@ -2973,22 +2984,22 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I45" t="s">
         <v>147</v>
@@ -3008,25 +3019,37 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="D46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E46" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="G46" t="s">
-        <v>53</v>
-      </c>
-      <c r="H46" t="b">
-        <v>0</v>
+        <v>102</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>147</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>100</v>
+      </c>
+      <c r="L46">
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -3037,34 +3060,22 @@
         <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>120</v>
+        <v>49</v>
       </c>
       <c r="D47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E47" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="G47" t="s">
-        <v>115</v>
-      </c>
-      <c r="H47">
-        <v>30</v>
-      </c>
-      <c r="I47" t="s">
-        <v>147</v>
-      </c>
-      <c r="J47">
-        <v>7</v>
-      </c>
-      <c r="K47">
-        <v>30</v>
-      </c>
-      <c r="L47">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -3075,34 +3086,34 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="D48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H48">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="I48" t="s">
         <v>147</v>
       </c>
       <c r="J48">
+        <v>7</v>
+      </c>
+      <c r="K48">
+        <v>30</v>
+      </c>
+      <c r="L48">
         <v>1</v>
-      </c>
-      <c r="K48">
-        <v>24</v>
-      </c>
-      <c r="L48">
-        <v>0.5</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -3113,34 +3124,34 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H49">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="I49" t="s">
         <v>147</v>
       </c>
       <c r="J49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="L49">
-        <v>10</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3151,19 +3162,19 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H50">
         <v>50</v>
@@ -3189,19 +3200,19 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H51">
         <v>50</v>
@@ -3219,7 +3230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="31.2">
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -3227,34 +3238,34 @@
         <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D52" t="s">
-        <v>207</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>142</v>
+        <v>206</v>
+      </c>
+      <c r="E52" t="s">
+        <v>119</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>155</v>
+        <v>119</v>
+      </c>
+      <c r="G52" t="s">
+        <v>119</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="I52" t="s">
         <v>147</v>
       </c>
       <c r="J52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="L52">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="31.2">
@@ -3265,28 +3276,28 @@
         <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D53" t="s">
-        <v>208</v>
-      </c>
-      <c r="E53" t="s">
-        <v>153</v>
+        <v>207</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I53" t="s">
         <v>147</v>
       </c>
       <c r="J53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K53">
         <v>36</v>
@@ -3303,33 +3314,71 @@
         <v>48</v>
       </c>
       <c r="C54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D54" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I54" t="s">
         <v>147</v>
       </c>
       <c r="J54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K54">
         <v>36</v>
       </c>
       <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="31.2">
+      <c r="A55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" t="s">
+        <v>209</v>
+      </c>
+      <c r="E55" t="s">
+        <v>154</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H55">
+        <v>3</v>
+      </c>
+      <c r="I55" t="s">
+        <v>147</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <v>36</v>
+      </c>
+      <c r="L55">
         <v>1</v>
       </c>
     </row>

</xml_diff>